<commit_message>
basic learning frameworks for label spreading and ladder nets, with some added file-reading functionality for LDA
</commit_message>
<xml_diff>
--- a/data/raw/postbatch90.xlsx
+++ b/data/raw/postbatch90.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>postCategory</t>
   </si>
@@ -77,52 +77,14 @@
     <t>3235930522</t>
   </si>
   <si>
-    <t xml:space="preserve">
-              ☎️(323) 593-0522   
-🍀🍀🍀🍀 GREENLEAF  THERAPY 🍀🍀🍀🍀   
-7203 GREENLEAF AVE WHITTIER, CALIFORNIA 90620   
-🍀☛(SUITE #H )🍀 ☛(SUITE #H )🍀☛(SUITE #H )   
-☎️(323) 593-0522   
-🍀CHICAS BELLAS ! LAS TERAPISTAS MÁS HERMOSAS    
-🍀VEN A CONOCERNOS    
-🍀TODO LO QUE KIERAS    
-🍀HABLAMOS ESPAÑOL !!!   
-🍀CLEAN    
-🍀PRIVATE   
-🍀EVERYTHING   
-🍀🍀JOVENES- HERMOSAS- COMPLACIENTES🍀🍀    
-🍀Beautiful Latinas ! READY TO SATISFY YOUR NEEDS!   
- 🍀🍀🍀OPEN FROM 9:30AM-LATE 🍀🍀🍀   
-🍀🍀🍀OPEN 7 DAYS A WEEK 🍀🍀🍀
-      </t>
-  </si>
-  <si>
-    <t>1209</t>
+    <t xml:space="preserve">
+              ☎️(323) 593-0522  </t>
   </si>
   <si>
     <t>🖤▃NEW❤ 9/3 ▃ 🖤LATINA GIRLS🖤▃▃▃▃❤▃▃▃ 🖤50×1HR🖤▃▃▃▃❤▃▃▃▃ 🖤50×1HR🖤▃▃▃▃❤▃▃▃▃ 🖤GRAND OPENING 🖤▃▃▃</t>
   </si>
   <si>
     <t>2017</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>119050048</t>
-  </si>
-  <si>
-    <t>Downtown, Los Angeles, Outcall Only</t>
-  </si>
-  <si>
-    <t>6267225855 2138055662</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-              Hey Guys!     I am Ivy, 23 years old.     I am a Taiwanese girl, 5'5", 103 lbs, 32C-23-34.     Call Only : 626-722-5855     Text Only : 213-805-5662</t>
-  </si>
-  <si>
-    <t>▊╳╳▊Asian ▊╳╳▊ Sexy▊╳╳▊⬛Anywhere out to you ▊╳╳▊ New Face▊╳╳▊Fantastic ▊╳╳▊ 626-722-5855 ▊╳╳▊╳╳▊╳╳▊╳</t>
   </si>
 </sst>
 </file>
@@ -471,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,40 +442,40 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="1" t="s">
+      <c s="1" r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c s="1" r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c s="1" r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c s="1" r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c s="1" r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c s="1" r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c s="1" r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c s="1" r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c s="1" r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c s="1" r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c s="1" r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c s="1" r="L1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -545,52 +507,14 @@
       <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="n">
+        <v>2333</v>
+      </c>
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" t="n">
-        <v>2335</v>
-      </c>
-      <c r="K3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>